<commit_message>
Add Lojban Crash Course Lesson 4 data
</commit_message>
<xml_diff>
--- a/data/crashcourse.xlsx
+++ b/data/crashcourse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Lesson1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="697">
   <si>
     <t>lo mlatu cu pinxe lo ladru</t>
   </si>
@@ -1400,12 +1400,836 @@
   <si>
     <t>I live near a shop.</t>
   </si>
+  <si>
+    <t>do ko'oi bajra</t>
+  </si>
+  <si>
+    <t>Run!</t>
+  </si>
+  <si>
+    <t>ko bajra</t>
+  </si>
+  <si>
+    <t>Do run!</t>
+  </si>
+  <si>
+    <t>nelci ko</t>
+  </si>
+  <si>
+    <t>Make it so you are liked by someone!</t>
+  </si>
+  <si>
+    <t>do ko'oi kurji do ko'oi</t>
+  </si>
+  <si>
+    <t>Take care of yourself.</t>
+  </si>
+  <si>
+    <t>ko kurji ko</t>
+  </si>
+  <si>
+    <t>mi'ai ko'oi klama</t>
+  </si>
+  <si>
+    <t>Let's go.</t>
+  </si>
+  <si>
+    <t>ko'oi klama</t>
+  </si>
+  <si>
+    <t>.e'o do lebna lo cukta</t>
+  </si>
+  <si>
+    <t>Could you take the book, please?</t>
+  </si>
+  <si>
+    <t>ko sutra bajra</t>
+  </si>
+  <si>
+    <t>Run quickly!</t>
+  </si>
+  <si>
+    <t>.e'o do pinxe lo tcati</t>
+  </si>
+  <si>
+    <t>Please, drink tea!</t>
+  </si>
+  <si>
+    <t>ko catlu lo skina</t>
+  </si>
+  <si>
+    <t>Watch a film!</t>
+  </si>
+  <si>
+    <t>Be smart!</t>
+  </si>
+  <si>
+    <t>ko stati</t>
+  </si>
+  <si>
+    <t>Go home!</t>
+  </si>
+  <si>
+    <t>ko klama lo zdani</t>
+  </si>
+  <si>
+    <t>Please, drink coffee!</t>
+  </si>
+  <si>
+    <t>.e'o do pinxe lo ckafi</t>
+  </si>
+  <si>
+    <t>Please, take care of the child.</t>
+  </si>
+  <si>
+    <t>.e'o do kurji lo verba</t>
+  </si>
+  <si>
+    <t>lo melbi je cmalu zdani</t>
+  </si>
+  <si>
+    <t>A pretty and small home is here.</t>
+  </si>
+  <si>
+    <t>lo melbi cmalu zdani cu zvati</t>
+  </si>
+  <si>
+    <t>A prettily small home is here.</t>
+  </si>
+  <si>
+    <t>mi .e do nelci lo jisra</t>
+  </si>
+  <si>
+    <t>I like juice, and you like juice.</t>
+  </si>
+  <si>
+    <t>mi je do nelci lo plise</t>
+  </si>
+  <si>
+    <t>I like apples, and you like apples.</t>
+  </si>
+  <si>
+    <t>mi nelci lo plise je lo jisra</t>
+  </si>
+  <si>
+    <t>I like apples and juice.</t>
+  </si>
+  <si>
+    <t>lo verba cu fengu ja bilma</t>
+  </si>
+  <si>
+    <t>The child is angry or ill </t>
+  </si>
+  <si>
+    <t>lo karce cu blabi jo nai grusi</t>
+  </si>
+  <si>
+    <t>The car is either white or gray.</t>
+  </si>
+  <si>
+    <t>mi prami do .i ju do fenki</t>
+  </si>
+  <si>
+    <t>I love you. Whether or not you are crazy.</t>
+  </si>
+  <si>
+    <t>lo nanla ce lo nixli cu klama lo panku</t>
+  </si>
+  <si>
+    <t>A boy with a girl go to a park.</t>
+  </si>
+  <si>
+    <t>lo nanla e lo nixli cu klama lo panka</t>
+  </si>
+  <si>
+    <t>A boy goes to a park, and a girl goes to a park.</t>
+  </si>
+  <si>
+    <t>lo nanla ce lo nixli cu casnu lo karce</t>
+  </si>
+  <si>
+    <t>A boy and a girl discuss a car.</t>
+  </si>
+  <si>
+    <t>lo nanla e lo nixli cu casnu lo karce</t>
+  </si>
+  <si>
+    <t>A boy discusses a car, and a girl discusses a car.</t>
+  </si>
+  <si>
+    <t>lo nanla ce nixli cu casnu lo karce</t>
+  </si>
+  <si>
+    <t>Someone who is a boy and a girl discusses a car.</t>
+  </si>
+  <si>
+    <t>mi nelci lo badna .e lo plise</t>
+  </si>
+  <si>
+    <t>I like bananas, and I like apples.</t>
+  </si>
+  <si>
+    <t>do sutra ja stati</t>
+  </si>
+  <si>
+    <t>You are quick or smart or both.</t>
+  </si>
+  <si>
+    <t>lo za'u prenu cu casnu lo karce .u lo gerku</t>
+  </si>
+  <si>
+    <t>The people discuss cars whether or not (they discuss) dogs.</t>
+  </si>
+  <si>
+    <t>mi citka lo najnimre .o nai lo badna</t>
+  </si>
+  <si>
+    <t>I eat either oranges or bananas.</t>
+  </si>
+  <si>
+    <t>Females like rain, and males like rain.</t>
+  </si>
+  <si>
+    <t>lo fetsi .e lo nakni cu nelci lo carvi</t>
+  </si>
+  <si>
+    <t>Either I or you go to the market.</t>
+  </si>
+  <si>
+    <t>mi .onai do klama lo zarci</t>
+  </si>
+  <si>
+    <t>I see a big and beautiful car.</t>
+  </si>
+  <si>
+    <t>mi viska lo barda je melbi karce</t>
+  </si>
+  <si>
+    <t>The child drinks milk and/or juice.</t>
+  </si>
+  <si>
+    <t>lo verba cu pinxe lo ladru .a lo jisra</t>
+  </si>
+  <si>
+    <t>The child and someone small discuss a car.</t>
+  </si>
+  <si>
+    <r>
+      <t>lo verba ce lo cmalu cu casnu lo pa karce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>lo najnimre cu barda i je ku'i lo badna cu cmalu</t>
+  </si>
+  <si>
+    <t>Oranges are big. But bananas are small.</t>
+  </si>
+  <si>
+    <t>lo nicte cu nu mi viska lo lunra</t>
+  </si>
+  <si>
+    <t>The night is when I see the Moon.</t>
+  </si>
+  <si>
+    <t>mi gleki lo nu do klama</t>
+  </si>
+  <si>
+    <t>I'm happy because you are coming.</t>
+  </si>
+  <si>
+    <t>mi djica lo nu do klama ti</t>
+  </si>
+  <si>
+    <t>I want you to come here (to this place)</t>
+  </si>
+  <si>
+    <t>lo cabna cu nicte</t>
+  </si>
+  <si>
+    <t>Now it's night. At present it's night.</t>
+  </si>
+  <si>
+    <t>lo nu pinxe lo ladru cu nabmi mi</t>
+  </si>
+  <si>
+    <t>Drinking milk is a problem, problematic to me.</t>
+  </si>
+  <si>
+    <t>mi nelci lo nu do dansu</t>
+  </si>
+  <si>
+    <t>I like you dancing.</t>
+  </si>
+  <si>
+    <t>xu do gleki lo nu do pilno lo skami</t>
+  </si>
+  <si>
+    <t>Are you happy of using a computer?</t>
+  </si>
+  <si>
+    <t>do djica lo nu mi citka lo plise xu</t>
+  </si>
+  <si>
+    <r>
+      <t>Do you want me to eat </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>an apple</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>Coming here is a problem.</t>
+  </si>
+  <si>
+    <t>lo nu klama ti cu nabmi</t>
+  </si>
+  <si>
+    <t>I want you to be happy.</t>
+  </si>
+  <si>
+    <t>mi djica lo nu do gleki</t>
+  </si>
+  <si>
+    <t>mi pinxe ca lo nu do klama</t>
+  </si>
+  <si>
+    <t>I drink while you are coming.</t>
+  </si>
+  <si>
+    <t>mi citka ba lo nu mi dansu</t>
+  </si>
+  <si>
+    <t>I eat after I dance.</t>
+  </si>
+  <si>
+    <t>lo mlatu ca pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats drink milk (at present).</t>
+  </si>
+  <si>
+    <t>lo mlatu pu pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats drank milk.</t>
+  </si>
+  <si>
+    <t>lo mlatu ba pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats will drink milk.</t>
+  </si>
+  <si>
+    <t>lo nicte cu pluka</t>
+  </si>
+  <si>
+    <t>The night is pleasant.</t>
+  </si>
+  <si>
+    <t>ba lo nicte cu pluka</t>
+  </si>
+  <si>
+    <t>After the night it is pleasant.</t>
+  </si>
+  <si>
+    <t>The night will be pleasant.</t>
+  </si>
+  <si>
+    <t>lo nicte cu ba pluka</t>
+  </si>
+  <si>
+    <t>mi pu citka ba lo nu mi dansu</t>
+  </si>
+  <si>
+    <t>I ate after I danced.</t>
+  </si>
+  <si>
+    <t>mi pu co'a cikna</t>
+  </si>
+  <si>
+    <t>I woke up</t>
+  </si>
+  <si>
+    <t>lo mlatu ca ca'o pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats (at present) are drinking milk.</t>
+  </si>
+  <si>
+    <t>lo mlatu ca mo'u pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats have drunk milk.</t>
+  </si>
+  <si>
+    <t>lo mlatu ca ta'e pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats (habitually, sometimes) drink milk.</t>
+  </si>
+  <si>
+    <t>lo mlatu pu mo'u pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats had drunk milk.</t>
+  </si>
+  <si>
+    <t>lo mlatu ba mo'u pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>Cats will have drunk milk.</t>
+  </si>
+  <si>
+    <t>mi pu ze'a sipna</t>
+  </si>
+  <si>
+    <t>I slept for a while.</t>
+  </si>
+  <si>
+    <t>mi pu sipna ze'a lo nicte</t>
+  </si>
+  <si>
+    <t>I slept through the night. I slept all night.</t>
+  </si>
+  <si>
+    <t>mi pu sipna ze'i lo nicte</t>
+  </si>
+  <si>
+    <t>I slept through the short night.</t>
+  </si>
+  <si>
+    <t>mi pu sipna ca lo nicte</t>
+  </si>
+  <si>
+    <t>I slept at night.</t>
+  </si>
+  <si>
+    <t>mi pinxe ri'a lo nu mi taske</t>
+  </si>
+  <si>
+    <t>I drink because I am thirsty.</t>
+  </si>
+  <si>
+    <t>mi citka ri'a lo nu mi xagji</t>
+  </si>
+  <si>
+    <t>I eat because I am hungry.</t>
+  </si>
+  <si>
+    <t>mi klama fa'a do to'o lo mlatu</t>
+  </si>
+  <si>
+    <t>I go to you from a cat.</t>
+  </si>
+  <si>
+    <t>mi cadzu bu'u lo tcadu</t>
+  </si>
+  <si>
+    <t>I walk in the city.</t>
+  </si>
+  <si>
+    <t>lo pa mlatu cu plipe fa'a mi ca lo nu do ca'o klama</t>
+  </si>
+  <si>
+    <t>A cat jumps towards me when you are coming.</t>
+  </si>
+  <si>
+    <r>
+      <t>lo pa mlatu cu plipe ca lo nu do ca'o klama </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>vau</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> fa'a mi</t>
+    </r>
+  </si>
+  <si>
+    <t>A cat jumps (when you are coming) towards me.</t>
+  </si>
+  <si>
+    <t>lo pa mlatu cu plipe ca lo nu do ca'o klama fa'a mi</t>
+  </si>
+  <si>
+    <t>A cat jumps (when you are coming towards me).</t>
+  </si>
+  <si>
+    <t>mi ca gleki lo nu do viska lo tsani</t>
+  </si>
+  <si>
+    <t>I am happy that you see the sky.</t>
+  </si>
+  <si>
+    <t>xu lo mlatu pu ca'o zvati lo zdani</t>
+  </si>
+  <si>
+    <t>Were cats staying at home?</t>
+  </si>
+  <si>
+    <t>do pu citka lo plise ba lo nu mi pinxe lo ladru</t>
+  </si>
+  <si>
+    <t>You ate an apple after I drank the milk.</t>
+  </si>
+  <si>
+    <t>ko catlu fa'a lo canko</t>
+  </si>
+  <si>
+    <t>Look towards the window.</t>
+  </si>
+  <si>
+    <t>xu do gleki ca lo nu do ca'o cadzu bu'u lo purdi</t>
+  </si>
+  <si>
+    <t>Are you happy when you are walking in the garden?</t>
+  </si>
+  <si>
+    <t>ca lo nu mi klama lo zdani vau do pinxe lo tcati ri'a lo nu do taske</t>
+  </si>
+  <si>
+    <t>When I go home you drink tea because you are thirsty.</t>
+  </si>
+  <si>
+    <t>You will see the sun.</t>
+  </si>
+  <si>
+    <t>do ba viska lo solri</t>
+  </si>
+  <si>
+    <t>You understand that it will rain.</t>
+  </si>
+  <si>
+    <t>do ca jimpe lo nu ba carvi</t>
+  </si>
+  <si>
+    <t>Quickly run away from the fire!</t>
+  </si>
+  <si>
+    <t>ko sutra bajra to'o lo fagri</t>
+  </si>
+  <si>
+    <t>We were staying at home when it was raining.</t>
+  </si>
+  <si>
+    <t>mi'ai pu ca'o zvati lo zdani ca lo nu carvi</t>
+  </si>
+  <si>
+    <t>mi na nelci do</t>
+  </si>
+  <si>
+    <t>I don't like you.</t>
+  </si>
+  <si>
+    <t>mi ja'a nelci do</t>
+  </si>
+  <si>
+    <t>I do like you.</t>
+  </si>
+  <si>
+    <t>la .bob. cu tcidu</t>
+  </si>
+  <si>
+    <t>Bob reads/is reading.</t>
+  </si>
+  <si>
+    <t>la .bob.djonson. cu tcidu</t>
+  </si>
+  <si>
+    <t>Bob Johnson reads/is reading.</t>
+  </si>
+  <si>
+    <t>la .lojban. cu bangu mi</t>
+  </si>
+  <si>
+    <t>I speak Lojban.</t>
+  </si>
+  <si>
+    <t>la .alis.</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>la .meilis.</t>
+  </si>
+  <si>
+    <t>Mei Li</t>
+  </si>
+  <si>
+    <t>la .bob.</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>la .abdul.</t>
+  </si>
+  <si>
+    <t>Abdul</t>
+  </si>
+  <si>
+    <t>la .ian.</t>
+  </si>
+  <si>
+    <r>
+      <t>Yan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ian</t>
+    </r>
+  </si>
+  <si>
+    <t>la .al.</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>la .doris.</t>
+  </si>
+  <si>
+    <t>Doris</t>
+  </si>
+  <si>
+    <t>la .micel.</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>la .kevin.</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>la .edvard.</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>la .adam.</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>la .lukas.</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>la alis cu klama lo zarci i le fetsi cu xagji</t>
+  </si>
+  <si>
+    <t>Alice is going to a shop. She is hungry.</t>
+  </si>
+  <si>
+    <t>la alis cu viska la doris i le fetsi cu melbi</t>
+  </si>
+  <si>
+    <t>Alice can see Doris. She (Doris) is beautiful.</t>
+  </si>
+  <si>
+    <t>coi do</t>
+  </si>
+  <si>
+    <t>Hello you.</t>
+  </si>
+  <si>
+    <t>cerni coi</t>
+  </si>
+  <si>
+    <t>Good morning!</t>
+  </si>
+  <si>
+    <t>vanci coi</t>
+  </si>
+  <si>
+    <t>Good evening!</t>
+  </si>
+  <si>
+    <t>donri coi</t>
+  </si>
+  <si>
+    <t>Good day!</t>
+  </si>
+  <si>
+    <t>nicte coi</t>
+  </si>
+  <si>
+    <t>Nightly greetings!</t>
+  </si>
+  <si>
+    <t>nicte co'o</t>
+  </si>
+  <si>
+    <t>Goodnight!</t>
+  </si>
+  <si>
+    <t>pluka nicte di'ai</t>
+  </si>
+  <si>
+    <t>Pleasant night!</t>
+  </si>
+  <si>
+    <t>di'ai do</t>
+  </si>
+  <si>
+    <t>Good luck to you!</t>
+  </si>
+  <si>
+    <t>mi'e la .doris.</t>
+  </si>
+  <si>
+    <t>I'm Doris. This is Doris speaking.</t>
+  </si>
+  <si>
+    <t>mi cliva doi la .robert.</t>
+  </si>
+  <si>
+    <t>I'm leaving, Robert.</t>
+  </si>
+  <si>
+    <t>mi cliva la .robert.</t>
+  </si>
+  <si>
+    <t>I'm leaving Robert.</t>
+  </si>
+  <si>
+    <t>ki'e do do pu sidju mi</t>
+  </si>
+  <si>
+    <t>je'e do</t>
+  </si>
+  <si>
+    <t>Thank you, you helped me.</t>
+  </si>
+  <si>
+    <t>Not at all.</t>
+  </si>
+  <si>
+    <t>coi .i xu do kanro</t>
+  </si>
+  <si>
+    <t>Hello. How do you do?</t>
+  </si>
+  <si>
+    <t>coi do mi djica lo nu do sidju mi</t>
+  </si>
+  <si>
+    <t>Hello. I want you to help me.</t>
+  </si>
+  <si>
+    <t>coi do la .alis. la .doris. pu cliva</t>
+  </si>
+  <si>
+    <t>Hello! Alice left Doris.</t>
+  </si>
+  <si>
+    <t>coi la .alis. la .doris. pu cliva</t>
+  </si>
+  <si>
+    <t>Hello, Alice! Doris's just left.</t>
+  </si>
+  <si>
+    <t>.ui coi do la .alis. la .doris. pu cliva</t>
+  </si>
+  <si>
+    <t>Yay, Hello! Alice left Doris.</t>
+  </si>
+  <si>
+    <t>cerni coi la .alis.</t>
+  </si>
+  <si>
+    <t>Good morning, Alice.</t>
+  </si>
+  <si>
+    <t>mi'e la .adam. i mi nelci lo nu mi ca'o tavla do</t>
+  </si>
+  <si>
+    <t>I am Adam. I like that I am talking to you.</t>
+  </si>
+  <si>
+    <t>mi ba sipna</t>
+  </si>
+  <si>
+    <t>I will sleep.</t>
+  </si>
+  <si>
+    <t>Good night.</t>
+  </si>
+  <si>
+    <t>Mommy, I will eat an apple.</t>
+  </si>
+  <si>
+    <t>doi lo mamta mi ba citka lo plise</t>
+  </si>
+  <si>
+    <t>You leave? Goodbye.</t>
+  </si>
+  <si>
+    <t>xu do cliva .i co'o do</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1453,6 +2277,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1471,7 +2302,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1559,8 +2390,60 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1569,8 +2452,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1614,6 +2498,32 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1657,6 +2567,32 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1986,10 +2922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2708,6 +3644,1039 @@
       </c>
       <c r="B88" s="2" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="17">
+      <c r="A89" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="17">
+      <c r="A90" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="17">
+      <c r="A91" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="17">
+      <c r="A92" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="17">
+      <c r="A93" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="17">
+      <c r="A94" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="17">
+      <c r="A95" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="17">
+      <c r="A96" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="17">
+      <c r="A97" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="17">
+      <c r="A98" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="17">
+      <c r="A99" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="17">
+      <c r="A100" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="17">
+      <c r="A101" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="17">
+      <c r="A102" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="17">
+      <c r="A103" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="17">
+      <c r="A104" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="17">
+      <c r="A105" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="17">
+      <c r="A106" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="17">
+      <c r="A107" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="17">
+      <c r="A108" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="17">
+      <c r="A109" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="17">
+      <c r="A110" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="17">
+      <c r="A111" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="17">
+      <c r="A112" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="17">
+      <c r="A113" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="17">
+      <c r="A114" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="17">
+      <c r="A115" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="17">
+      <c r="A116" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="17">
+      <c r="A117" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="17">
+      <c r="A118" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="17">
+      <c r="A119" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="17">
+      <c r="A120" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="17">
+      <c r="A121" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="17">
+      <c r="A122" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="17">
+      <c r="A123" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="17">
+      <c r="A124" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="17">
+      <c r="A125" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="17">
+      <c r="A126" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="17">
+      <c r="A127" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="17">
+      <c r="A128" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="17">
+      <c r="A129" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="17">
+      <c r="A130" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="17">
+      <c r="A131" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="17">
+      <c r="A132" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="17">
+      <c r="A133" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="17">
+      <c r="A134" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="17">
+      <c r="A135" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="17">
+      <c r="A136" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="17">
+      <c r="A137" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="17">
+      <c r="A138" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="17">
+      <c r="A139" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="17">
+      <c r="A140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="17">
+      <c r="A141" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="17">
+      <c r="A142" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="17">
+      <c r="A143" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="17">
+      <c r="A144" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="17">
+      <c r="A145" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="17">
+      <c r="A146" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="17">
+      <c r="A147" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="17">
+      <c r="A148" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="17">
+      <c r="A149" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="17">
+      <c r="A150" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="17">
+      <c r="A151" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="17">
+      <c r="A152" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="17">
+      <c r="A153" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="17">
+      <c r="A154" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="17">
+      <c r="A155" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="17">
+      <c r="A156" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="17" customHeight="1">
+      <c r="A157" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="17">
+      <c r="A158" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="17">
+      <c r="A159" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="17">
+      <c r="A160" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="17">
+      <c r="A161" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="17">
+      <c r="A162" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="17">
+      <c r="A163" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="17">
+      <c r="A164" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="17">
+      <c r="A165" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="17">
+      <c r="A166" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="17">
+      <c r="A167" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="17">
+      <c r="A168" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="17">
+      <c r="A169" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="17">
+      <c r="A170" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="17">
+      <c r="A171" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="17">
+      <c r="A172" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="17">
+      <c r="A173" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="17">
+      <c r="A174" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="17">
+      <c r="A175" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="17">
+      <c r="A176" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="17">
+      <c r="A177" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="17">
+      <c r="A178" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="17">
+      <c r="A179" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="17">
+      <c r="A180" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C180" s="5"/>
+    </row>
+    <row r="181" spans="1:3" ht="17">
+      <c r="A181" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="17">
+      <c r="A182" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="17">
+      <c r="A183" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="17">
+      <c r="A184" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="17">
+      <c r="A185" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="17">
+      <c r="A186" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="17">
+      <c r="A187" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="17">
+      <c r="A188" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="17">
+      <c r="A189" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="17">
+      <c r="A190" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="17">
+      <c r="A191" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="17">
+      <c r="A192" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="17">
+      <c r="A193" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="17">
+      <c r="A194" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="17">
+      <c r="A195" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="17">
+      <c r="A196" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="17">
+      <c r="A197" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="17">
+      <c r="A198" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="17">
+      <c r="A199" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="17">
+      <c r="A200" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="17">
+      <c r="A201" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="17">
+      <c r="A202" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="17">
+      <c r="A203" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="17">
+      <c r="A204" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="17">
+      <c r="A205" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="17">
+      <c r="A206" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="17">
+      <c r="A207" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="17">
+      <c r="A208" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="17">
+      <c r="A209" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="17">
+      <c r="A210" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="17">
+      <c r="A211" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="17">
+      <c r="A212" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="17">
+      <c r="A213" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="17">
+      <c r="A214" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="17">
+      <c r="A215" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="17">
+      <c r="A216" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="17">
+      <c r="A217" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -2725,7 +4694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A127" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
@@ -3013,7 +4982,7 @@
       <c r="B32" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" ht="17">
       <c r="A33" s="1" t="s">
@@ -3022,7 +4991,7 @@
       <c r="B33" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3" ht="17">
       <c r="A34" s="1" t="s">
@@ -3031,7 +5000,7 @@
       <c r="B34" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3" ht="17">
       <c r="A35" s="1" t="s">
@@ -3067,7 +5036,7 @@
       <c r="B38" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" ht="17">
       <c r="A39" s="1" t="s">
@@ -3076,7 +5045,7 @@
       <c r="B39" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:3" ht="17">
       <c r="A40" s="1" t="s">

</xml_diff>

<commit_message>
Add jbo<->eng dictionary from Lojban Crash Course.
</commit_message>
<xml_diff>
--- a/data/crashcourse.xlsx
+++ b/data/crashcourse.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lesson1" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson4" sheetId="2" r:id="rId2"/>
+    <sheet name="jbo&lt;-&gt;eng dict" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="767">
   <si>
     <t>lo mlatu cu pinxe lo ladru</t>
   </si>
@@ -2223,6 +2224,216 @@
   </si>
   <si>
     <t>xu do cliva .i co'o do</t>
+  </si>
+  <si>
+    <t>ei mi tavla la alis a la kevin</t>
+  </si>
+  <si>
+    <t>I need to speak to Alice or Kevin (or to both of them).</t>
+  </si>
+  <si>
+    <t>a'a ko ca'o skicu</t>
+  </si>
+  <si>
+    <t>I'm listening, go on talking!</t>
+  </si>
+  <si>
+    <t>a'a cu'i ko denpa lo nu mi jai gau mulno fai ti</t>
+  </si>
+  <si>
+    <t>Eh, just a second, let me finish this.</t>
+  </si>
+  <si>
+    <t>do tavla da a'a nai</t>
+  </si>
+  <si>
+    <t>La, la, la, I'm not listening what you are talking about.</t>
+  </si>
+  <si>
+    <t>a'e ba vlile tcima</t>
+  </si>
+  <si>
+    <t>It's going to be a storm.</t>
+  </si>
+  <si>
+    <t>a'e nai mi ba klama lo ckana</t>
+  </si>
+  <si>
+    <t>Yaaaawn, I'm going to bed.</t>
+  </si>
+  <si>
+    <t>a'i mi ca'o ralte</t>
+  </si>
+  <si>
+    <t>I'm trying to hold it!</t>
+  </si>
+  <si>
+    <t>a'i cu'i ti frili</t>
+  </si>
+  <si>
+    <t>Ah, this is easy.</t>
+  </si>
+  <si>
+    <t>a'i nai cikre ta</t>
+  </si>
+  <si>
+    <t>Nah, why bother fixing it.</t>
+  </si>
+  <si>
+    <t>a'o vamji fa lo nu zukte</t>
+  </si>
+  <si>
+    <t>I hope, it's worth doing it.</t>
+  </si>
+  <si>
+    <t>a'o nai mi co'u ponse da</t>
+  </si>
+  <si>
+    <t>Gah, I lost all my property.</t>
+  </si>
+  <si>
+    <t>a'oi la kevin ma nuzba</t>
+  </si>
+  <si>
+    <t>Ahoy, Kevin! What's up?</t>
+  </si>
+  <si>
+    <t>a'u ro jbopre cu stati prenu</t>
+  </si>
+  <si>
+    <t>Interesting, all Lojbanists are smart people.</t>
+  </si>
+  <si>
+    <t>a'u ma krinu</t>
+  </si>
+  <si>
+    <t>Hm, what is the reason?</t>
+  </si>
+  <si>
+    <t>a'u cu'i do ne ka'ai lo nanla cu se zdani</t>
+  </si>
+  <si>
+    <t>It's none of my business that you live with a boy.</t>
+  </si>
+  <si>
+    <t>a'u nai do co'a speni lo fange</t>
+  </si>
+  <si>
+    <t>You married a stranger, it's none of my business, I'd avoid this topic.</t>
+  </si>
+  <si>
+    <t>a'u nai iu nai panci fa lo kalci i ai nai mi citka ti</t>
+  </si>
+  <si>
+    <t>Yuck, that smells like shit! I'm not going to eat this.</t>
+  </si>
+  <si>
+    <t>lo aftobuso</t>
+  </si>
+  <si>
+    <t>bus, coach.</t>
+  </si>
+  <si>
+    <t>ma se stuzi lo tcana pe lo aftobuso pe li mu</t>
+  </si>
+  <si>
+    <t>Where is the stop of bus number 5?</t>
+  </si>
+  <si>
+    <t>lo aftobuso pe li xo cu klama lo muzga</t>
+  </si>
+  <si>
+    <t>What's the number of the bus that goes to the museum?</t>
+  </si>
+  <si>
+    <t>lo aftobuso be lo litru cu clani</t>
+  </si>
+  <si>
+    <t>Tourists' bus is long.</t>
+  </si>
+  <si>
+    <t>ai mi vitke do</t>
+  </si>
+  <si>
+    <t>I'm going to visit you.</t>
+  </si>
+  <si>
+    <t>a'i cu'i mi klama lo zarci</t>
+  </si>
+  <si>
+    <t>I'm indecisive to whether I should go to a shop.</t>
+  </si>
+  <si>
+    <t>ai nai mi pu darxi do</t>
+  </si>
+  <si>
+    <t>I didn't mean to hit you.</t>
+  </si>
+  <si>
+    <t>lo se aidji</t>
+  </si>
+  <si>
+    <t>intended action.</t>
+  </si>
+  <si>
+    <t>mi aidji lo ka klama la nipon</t>
+  </si>
+  <si>
+    <t>I am going to go to Japan.</t>
+  </si>
+  <si>
+    <t>lo akti</t>
+  </si>
+  <si>
+    <t>in operation</t>
+  </si>
+  <si>
+    <t>lo se akti</t>
+  </si>
+  <si>
+    <t>active operation.</t>
+  </si>
+  <si>
+    <t>gau ko ta to'e akti</t>
+  </si>
+  <si>
+    <t>Turn that off.</t>
+  </si>
+  <si>
+    <t>gau ko ta akti</t>
+  </si>
+  <si>
+    <t>Turn it on.</t>
+  </si>
+  <si>
+    <t>mi jai gau ba akti fai le minji</t>
+  </si>
+  <si>
+    <t>I will get the machine running.</t>
+  </si>
+  <si>
+    <t>le zarci ca akti</t>
+  </si>
+  <si>
+    <t>The shop is open.</t>
+  </si>
+  <si>
+    <t>le minji ca akti lo ka cupra lo purmo</t>
+  </si>
+  <si>
+    <t>The machine is now in operation producing flour.</t>
+  </si>
+  <si>
+    <t>le verba pu jai gau spofu lo anka be lo no'a</t>
+  </si>
+  <si>
+    <t>The child broke his thigh.</t>
+  </si>
+  <si>
+    <t>lo ankabuta</t>
+  </si>
+  <si>
+    <t>spider</t>
   </si>
 </sst>
 </file>
@@ -2443,7 +2654,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2452,6 +2663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="139">
@@ -2924,7 +3136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A195" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
@@ -4982,7 +5194,7 @@
       <c r="B32" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="17">
       <c r="A33" s="1" t="s">
@@ -4991,7 +5203,7 @@
       <c r="B33" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" ht="17">
       <c r="A34" s="1" t="s">
@@ -5000,7 +5212,7 @@
       <c r="B34" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" ht="17">
       <c r="A35" s="1" t="s">
@@ -5036,7 +5248,7 @@
       <c r="B38" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="8"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" ht="17">
       <c r="A39" s="1" t="s">
@@ -5045,7 +5257,7 @@
       <c r="B39" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="1:3" ht="17">
       <c r="A40" s="1" t="s">
@@ -5974,4 +6186,307 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="55.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17">
+      <c r="A1" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17">
+      <c r="A2" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17">
+      <c r="A3" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17">
+      <c r="A4" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17">
+      <c r="A5" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17">
+      <c r="A6" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17">
+      <c r="A7" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17">
+      <c r="A8" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17">
+      <c r="A9" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17">
+      <c r="A10" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17">
+      <c r="A11" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17">
+      <c r="A12" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17">
+      <c r="A13" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17">
+      <c r="A14" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17">
+      <c r="A15" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17">
+      <c r="A16" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17">
+      <c r="A17" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17">
+      <c r="A18" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17">
+      <c r="A19" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17">
+      <c r="A20" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17">
+      <c r="A21" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17">
+      <c r="A22" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17">
+      <c r="A23" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17">
+      <c r="A24" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17">
+      <c r="A25" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17">
+      <c r="A26" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17">
+      <c r="A27" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17">
+      <c r="A28" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17">
+      <c r="A29" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17">
+      <c r="A30" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17">
+      <c r="A31" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17">
+      <c r="A32" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="17">
+      <c r="A33" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17">
+      <c r="A34" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17">
+      <c r="A35" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>766</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>